<commit_message>
finalized party vessels catch and anglers effort data
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb111/raw/Table22.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb111/raw/Table22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb111/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052AE112-6B08-864E-A2D1-53861CDFF85E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0706028A-03E2-174E-9744-41F140A769A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -142,23 +142,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -477,7 +477,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -884,7 +884,7 @@
         <v>556949</v>
       </c>
       <c r="D12" s="7">
-        <v>588067</v>
+        <v>588087</v>
       </c>
       <c r="E12" s="7">
         <v>502146</v>

</xml_diff>